<commit_message>
separando as criações dos documentos
</commit_message>
<xml_diff>
--- a/docs/videos_transcrever.xlsx
+++ b/docs/videos_transcrever.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t xml:space="preserve">URL_VIDEO</t>
   </si>
@@ -31,10 +31,16 @@
     <t xml:space="preserve">FEITO</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.youtube.com/watch?v=bRKP73xnf30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ainda Vale a Pena Ser FREELANCER? PRÓS E CONTRAS</t>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=8MLqI-8xNcM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Windows 11 bloqueando pcs fora dos requisitos mínimos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.youtube.com/watch?v=hAeJDW281vY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Porque as pessoas gostam mais do Windows antigos?</t>
   </si>
 </sst>
 </file>
@@ -44,7 +50,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -65,6 +71,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -109,7 +122,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -120,6 +133,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -245,16 +262,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="41.49"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="62.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="43.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="87.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -278,6 +295,12 @@
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -285,6 +308,9 @@
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C5" s="2"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B6" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>